<commit_message>
add names to lines& buses +
dump the results to output folder
</commit_message>
<xml_diff>
--- a/input/busIn.xlsx
+++ b/input/busIn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GITHUB_PRIVATE_CODES\ForwardBackwardSweep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GITHUB_PRIVATE_CODES\advancedFBSweep\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E4E787-27FE-43FA-905E-3BC6D00B8ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A90413-C33C-416A-8E12-95A053DCE3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4FDC1957-8DB4-4927-B139-8B72076C7FCA}"/>
   </bookViews>
@@ -36,12 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="6">
   <si>
     <t>kW</t>
   </si>
   <si>
     <t>kVAR</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>lorem</t>
+  </si>
+  <si>
+    <t>ipsum</t>
+  </si>
+  <si>
+    <t>at</t>
   </si>
 </sst>
 </file>
@@ -394,283 +406,487 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C5F0F7-AFD7-4958-8DBE-6D4C4979D1E6}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>100</v>
       </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="D3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>90</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>120</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>60</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>60</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
       </c>
       <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>200</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <v>200</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>60</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
       </c>
       <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>60</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
       </c>
       <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
         <v>45</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>60</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
       </c>
       <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+      <c r="D13">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>60</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
       </c>
       <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
         <v>120</v>
       </c>
-      <c r="B15">
+      <c r="D15">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>60</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
       </c>
       <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>60</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
       </c>
       <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>60</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
       </c>
       <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
         <v>90</v>
       </c>
-      <c r="B19">
+      <c r="D19">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
         <v>90</v>
       </c>
-      <c r="B20">
+      <c r="D20">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
         <v>90</v>
       </c>
-      <c r="B21">
+      <c r="D21">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
         <v>90</v>
       </c>
-      <c r="B22">
+      <c r="D22">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
         <v>90</v>
       </c>
-      <c r="B23">
+      <c r="D23">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
         <v>90</v>
       </c>
-      <c r="B24">
+      <c r="D24">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
         <v>420</v>
       </c>
-      <c r="B25">
+      <c r="D25">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
         <v>420</v>
       </c>
-      <c r="B26">
+      <c r="D26">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>60</v>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
       </c>
       <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>60</v>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
       </c>
       <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>60</v>
+      </c>
+      <c r="D28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>60</v>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
       </c>
       <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>60</v>
+      </c>
+      <c r="D29">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
         <v>120</v>
       </c>
-      <c r="B30">
+      <c r="D30">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
         <v>200</v>
       </c>
-      <c r="B31">
+      <c r="D31">
         <v>600</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
         <v>150</v>
       </c>
-      <c r="B32">
+      <c r="D32">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
         <v>210</v>
       </c>
-      <c r="B33">
+      <c r="D33">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>60</v>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
       </c>
       <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34">
         <v>40</v>
       </c>
     </row>

</xml_diff>